<commit_message>
No se pudo lo de guardar cambios. Saludos
</commit_message>
<xml_diff>
--- a/Archivos/archivo1_657141be55ea1.xlsx
+++ b/Archivos/archivo1_657141be55ea1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>NÚMERO</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>VR2N</t>
+  </si>
+  <si>
+    <t>34e</t>
   </si>
   <si>
     <t>1R2</t>
@@ -3646,7 +3649,7 @@
   </sheetPr>
   <dimension ref="A1:AZ352"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="false" showRowColHeaders="1" topLeftCell="B1">
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="B1">
       <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
@@ -3839,10 +3842,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="52">
-        <v>2</v>
-      </c>
-      <c r="M2" s="52">
-        <v>3</v>
+        <v>23</v>
+      </c>
+      <c r="M2" s="52" t="s">
+        <v>23</v>
       </c>
       <c r="N2" s="52">
         <v>45</v>
@@ -3857,25 +3860,25 @@
         <v>18</v>
       </c>
       <c r="R2" s="52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S2" s="57" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="V2" s="52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="X2" s="52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Y2" s="52" t="s">
         <v>18</v>
@@ -3883,25 +3886,25 @@
       <c r="Z2" s="52"/>
       <c r="AA2" s="52"/>
       <c r="AB2" s="52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="AD2" s="52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AE2" s="52" t="s">
         <v>18</v>
       </c>
       <c r="AF2" s="52" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AG2" s="52" t="s">
         <v>21</v>
       </c>
       <c r="AH2" s="52" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI2" s="52" t="s">
         <v>21</v>
@@ -3909,7 +3912,7 @@
       <c r="AJ2" s="52"/>
       <c r="AK2" s="52"/>
       <c r="AL2" s="52" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM2" s="48" t="s">
         <v>21</v>
@@ -3944,13 +3947,13 @@
         <v>19</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3" s="57" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J3" s="57" t="s">
         <v>21</v>
@@ -3967,19 +3970,19 @@
         <v>18</v>
       </c>
       <c r="R3" s="52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S3" s="57" t="s">
         <v>18</v>
       </c>
       <c r="T3" s="52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U3" s="52" t="s">
         <v>18</v>
       </c>
       <c r="V3" s="52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="W3" s="52" t="s">
         <v>18</v>
@@ -3989,13 +3992,13 @@
       <c r="Z3" s="52"/>
       <c r="AA3" s="52"/>
       <c r="AB3" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC3" s="52" t="s">
         <v>18</v>
       </c>
       <c r="AD3" s="52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AE3" s="52" t="s">
         <v>21</v>
@@ -4042,13 +4045,13 @@
         <v>19</v>
       </c>
       <c r="G4" s="52" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H4" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="57" t="s">
         <v>21</v>
@@ -4065,13 +4068,13 @@
         <v>18</v>
       </c>
       <c r="R4" s="52" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S4" s="57" t="s">
         <v>18</v>
       </c>
       <c r="T4" s="52" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U4" s="52" t="s">
         <v>18</v>
@@ -4083,7 +4086,7 @@
       <c r="Z4" s="52"/>
       <c r="AA4" s="52"/>
       <c r="AB4" s="52" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC4" s="52" t="s">
         <v>21</v>
@@ -4122,7 +4125,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="48" t="s">
@@ -4132,7 +4135,7 @@
         <v>19</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H5" s="52" t="s">
         <v>18</v>
@@ -4143,7 +4146,7 @@
       <c r="L5" s="52"/>
       <c r="M5" s="52"/>
       <c r="N5" s="53" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="O5" s="52" t="s">
         <v>18</v>
@@ -4151,13 +4154,13 @@
       <c r="P5" s="52"/>
       <c r="Q5" s="52"/>
       <c r="R5" s="52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S5" s="57" t="s">
         <v>18</v>
       </c>
       <c r="T5" s="52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U5" s="52" t="s">
         <v>18</v>
@@ -4169,7 +4172,7 @@
       <c r="Z5" s="52"/>
       <c r="AA5" s="52"/>
       <c r="AB5" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC5" s="52" t="s">
         <v>18</v>
@@ -4179,7 +4182,7 @@
       <c r="AF5" s="52"/>
       <c r="AG5" s="52"/>
       <c r="AH5" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI5" s="52" t="s">
         <v>18</v>
@@ -4212,7 +4215,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="48" t="s">
@@ -4222,7 +4225,7 @@
         <v>19</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H6" s="52" t="s">
         <v>18</v>
@@ -4237,7 +4240,7 @@
       <c r="P6" s="52"/>
       <c r="Q6" s="52"/>
       <c r="R6" s="52" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S6" s="57" t="s">
         <v>18</v>
@@ -4286,7 +4289,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="48" t="s">
@@ -4296,7 +4299,7 @@
         <v>19</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="52" t="s">
         <v>18</v>
@@ -4311,7 +4314,7 @@
       <c r="P7" s="52"/>
       <c r="Q7" s="52"/>
       <c r="R7" s="52" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S7" s="57" t="s">
         <v>18</v>
@@ -4360,7 +4363,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="48" t="s">
@@ -4370,7 +4373,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H8" s="52" t="s">
         <v>18</v>
@@ -4385,13 +4388,13 @@
       <c r="P8" s="52"/>
       <c r="Q8" s="52"/>
       <c r="R8" s="52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S8" s="57" t="s">
         <v>18</v>
       </c>
       <c r="T8" s="52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="U8" s="52" t="s">
         <v>18</v>
@@ -4438,7 +4441,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="48" t="s">
@@ -4448,7 +4451,7 @@
         <v>19</v>
       </c>
       <c r="G9" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" s="52" t="s">
         <v>18</v>
@@ -4504,7 +4507,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="48" t="s">
@@ -4514,7 +4517,7 @@
         <v>19</v>
       </c>
       <c r="G10" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H10" s="52" t="s">
         <v>21</v>
@@ -4539,7 +4542,7 @@
       <c r="Z10" s="52"/>
       <c r="AA10" s="52"/>
       <c r="AB10" s="52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC10" s="52" t="s">
         <v>21</v>
@@ -4574,7 +4577,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="48" t="s">
@@ -4584,13 +4587,13 @@
         <v>19</v>
       </c>
       <c r="G11" s="52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J11" s="52" t="s">
         <v>21</v>
@@ -4599,7 +4602,7 @@
       <c r="L11" s="52"/>
       <c r="M11" s="52"/>
       <c r="N11" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O11" s="52" t="s">
         <v>18</v>
@@ -4617,13 +4620,13 @@
       <c r="Z11" s="52"/>
       <c r="AA11" s="52"/>
       <c r="AB11" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC11" s="52" t="s">
         <v>21</v>
       </c>
       <c r="AD11" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE11" s="52" t="s">
         <v>21</v>
@@ -4656,7 +4659,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="48" t="s">
@@ -4666,7 +4669,7 @@
         <v>19</v>
       </c>
       <c r="G12" s="52" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="52" t="s">
         <v>21</v>
@@ -4677,7 +4680,7 @@
       <c r="L12" s="54"/>
       <c r="M12" s="52"/>
       <c r="N12" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O12" s="52" t="s">
         <v>21</v>
@@ -4726,7 +4729,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="11"/>
       <c r="E13" s="48" t="s">
@@ -4736,13 +4739,13 @@
         <v>19</v>
       </c>
       <c r="G13" s="52" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H13" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I13" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J13" s="57" t="s">
         <v>21</v>
@@ -4765,13 +4768,13 @@
       <c r="Z13" s="52"/>
       <c r="AA13" s="52"/>
       <c r="AB13" s="52" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC13" s="52" t="s">
         <v>21</v>
       </c>
       <c r="AD13" s="52" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AE13" s="52" t="s">
         <v>21</v>
@@ -4804,7 +4807,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="48" t="s">
@@ -4814,7 +4817,7 @@
         <v>19</v>
       </c>
       <c r="G14" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H14" s="52" t="s">
         <v>18</v>
@@ -4870,7 +4873,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="48" t="s">
@@ -4880,7 +4883,7 @@
         <v>19</v>
       </c>
       <c r="G15" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H15" s="52" t="s">
         <v>18</v>
@@ -4936,7 +4939,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D16" s="47"/>
       <c r="E16" s="48" t="s">
@@ -4946,7 +4949,7 @@
         <v>19</v>
       </c>
       <c r="G16" s="52" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H16" s="52" t="s">
         <v>18</v>
@@ -5002,7 +5005,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="48" t="s">
@@ -5012,13 +5015,13 @@
         <v>19</v>
       </c>
       <c r="G17" s="52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H17" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I17" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J17" s="52" t="s">
         <v>18</v>
@@ -5082,7 +5085,7 @@
         <v>19</v>
       </c>
       <c r="G18" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H18" s="52" t="s">
         <v>18</v>
@@ -5148,7 +5151,7 @@
         <v>19</v>
       </c>
       <c r="G19" s="48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H19" s="52" t="s">
         <v>18</v>
@@ -5204,7 +5207,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D20" s="47"/>
       <c r="E20" s="46" t="s">
@@ -5214,7 +5217,7 @@
         <v>19</v>
       </c>
       <c r="G20" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H20" s="52" t="s">
         <v>18</v>
@@ -5270,7 +5273,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D21" s="47"/>
       <c r="E21" s="46" t="s">
@@ -5280,7 +5283,7 @@
         <v>19</v>
       </c>
       <c r="G21" s="48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H21" s="52" t="s">
         <v>18</v>
@@ -5336,7 +5339,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" s="47"/>
       <c r="E22" s="46" t="s">
@@ -5346,13 +5349,13 @@
         <v>19</v>
       </c>
       <c r="G22" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H22" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I22" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J22" s="48" t="s">
         <v>18</v>
@@ -5361,7 +5364,7 @@
       <c r="L22" s="49"/>
       <c r="M22" s="48"/>
       <c r="N22" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O22" s="48" t="s">
         <v>18</v>
@@ -5379,13 +5382,13 @@
       <c r="Z22" s="48"/>
       <c r="AA22" s="48"/>
       <c r="AB22" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC22" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD22" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE22" s="48" t="s">
         <v>21</v>
@@ -5418,7 +5421,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D23" s="47"/>
       <c r="E23" s="46" t="s">
@@ -5428,7 +5431,7 @@
         <v>19</v>
       </c>
       <c r="G23" s="48" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H23" s="57" t="s">
         <v>21</v>
@@ -5453,7 +5456,7 @@
       <c r="Z23" s="48"/>
       <c r="AA23" s="48"/>
       <c r="AB23" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC23" s="48" t="s">
         <v>21</v>
@@ -5463,7 +5466,7 @@
       <c r="AF23" s="48"/>
       <c r="AG23" s="48"/>
       <c r="AH23" s="48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI23" s="48" t="s">
         <v>21</v>
@@ -5502,13 +5505,13 @@
         <v>19</v>
       </c>
       <c r="G24" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H24" s="57" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J24" s="46" t="s">
         <v>21</v>
@@ -5521,28 +5524,28 @@
       <c r="P24" s="48"/>
       <c r="Q24" s="48"/>
       <c r="R24" s="46" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S24" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="T24" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="T24" s="46" t="s">
-        <v>52</v>
-      </c>
       <c r="U24" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="V24" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="W24" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="X24" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="V24" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="W24" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="X24" s="46" t="s">
-        <v>52</v>
-      </c>
       <c r="Y24" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z24" s="48"/>
       <c r="AA24" s="48"/>
@@ -5592,13 +5595,13 @@
         <v>19</v>
       </c>
       <c r="G25" s="46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H25" s="46" t="s">
         <v>21</v>
       </c>
       <c r="I25" s="46" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J25" s="46" t="s">
         <v>21</v>
@@ -5615,10 +5618,10 @@
         <v>18</v>
       </c>
       <c r="R25" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="S25" s="46" t="s">
         <v>54</v>
-      </c>
-      <c r="S25" s="46" t="s">
-        <v>53</v>
       </c>
       <c r="T25" s="48"/>
       <c r="U25" s="48"/>
@@ -5629,7 +5632,7 @@
       <c r="Z25" s="48"/>
       <c r="AA25" s="48"/>
       <c r="AB25" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC25" s="46" t="s">
         <v>18</v>
@@ -5653,7 +5656,7 @@
       <c r="AP25" s="48"/>
       <c r="AQ25" s="55"/>
       <c r="AR25" s="59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AS25" s="58"/>
       <c r="AT25" s="58"/>
@@ -5680,7 +5683,7 @@
         <v>19</v>
       </c>
       <c r="G26" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>21</v>
@@ -5695,7 +5698,7 @@
       <c r="P26" s="48"/>
       <c r="Q26" s="48"/>
       <c r="R26" s="48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S26" s="48" t="s">
         <v>21</v>
@@ -5750,7 +5753,7 @@
         <v>19</v>
       </c>
       <c r="G27" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H27" s="52" t="s">
         <v>21</v>
@@ -5765,10 +5768,10 @@
       <c r="P27" s="48"/>
       <c r="Q27" s="48"/>
       <c r="R27" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="S27" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T27" s="48"/>
       <c r="U27" s="48"/>
@@ -5785,7 +5788,7 @@
       <c r="AF27" s="48"/>
       <c r="AG27" s="48"/>
       <c r="AH27" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI27" s="48" t="s">
         <v>18</v>
@@ -5803,7 +5806,7 @@
       <c r="AP27" s="48"/>
       <c r="AQ27" s="48"/>
       <c r="AR27" s="59" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AS27" s="13"/>
       <c r="AT27" s="13"/>
@@ -5830,13 +5833,13 @@
         <v>19</v>
       </c>
       <c r="G28" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H28" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J28" s="46" t="s">
         <v>21</v>
@@ -5853,16 +5856,16 @@
         <v>18</v>
       </c>
       <c r="R28" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S28" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="T28" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U28" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="V28" s="48"/>
       <c r="W28" s="48"/>
@@ -5871,7 +5874,7 @@
       <c r="Z28" s="48"/>
       <c r="AA28" s="48"/>
       <c r="AB28" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC28" s="48" t="s">
         <v>18</v>
@@ -5881,19 +5884,19 @@
       <c r="AF28" s="48"/>
       <c r="AG28" s="48"/>
       <c r="AH28" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AI28" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AJ28" s="48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AK28" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AL28" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM28" s="48" t="s">
         <v>18</v>
@@ -5907,7 +5910,7 @@
       <c r="AP28" s="48"/>
       <c r="AQ28" s="48"/>
       <c r="AR28" s="59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AS28" s="13"/>
       <c r="AT28" s="13"/>
@@ -5934,7 +5937,7 @@
         <v>19</v>
       </c>
       <c r="G29" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H29" s="52" t="s">
         <v>21</v>
@@ -5949,22 +5952,22 @@
       <c r="P29" s="48"/>
       <c r="Q29" s="48"/>
       <c r="R29" s="52" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S29" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="T29" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="T29" s="52" t="s">
-        <v>52</v>
-      </c>
       <c r="U29" s="46" t="s">
+        <v>54</v>
+      </c>
+      <c r="V29" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="V29" s="52" t="s">
-        <v>52</v>
-      </c>
       <c r="W29" s="46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="X29" s="48"/>
       <c r="Y29" s="48"/>
@@ -5977,13 +5980,13 @@
       <c r="AF29" s="48"/>
       <c r="AG29" s="48"/>
       <c r="AH29" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI29" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AJ29" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AK29" s="48" t="s">
         <v>18</v>
@@ -5995,7 +5998,7 @@
       <c r="AP29" s="48"/>
       <c r="AQ29" s="48"/>
       <c r="AR29" s="59" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AS29" s="13"/>
       <c r="AT29" s="13"/>
@@ -6022,7 +6025,7 @@
         <v>19</v>
       </c>
       <c r="G30" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H30" s="52" t="s">
         <v>21</v>
@@ -6037,7 +6040,7 @@
       <c r="P30" s="48"/>
       <c r="Q30" s="48"/>
       <c r="R30" s="48" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="S30" s="48" t="s">
         <v>18</v>
@@ -6092,7 +6095,7 @@
         <v>19</v>
       </c>
       <c r="G31" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H31" s="52" t="s">
         <v>21</v>
@@ -6103,7 +6106,7 @@
       <c r="L31" s="49"/>
       <c r="M31" s="48"/>
       <c r="N31" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O31" s="48" t="s">
         <v>21</v>
@@ -6111,7 +6114,7 @@
       <c r="P31" s="48"/>
       <c r="Q31" s="48"/>
       <c r="R31" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S31" s="48" t="s">
         <v>18</v>
@@ -6125,7 +6128,7 @@
       <c r="Z31" s="48"/>
       <c r="AA31" s="48"/>
       <c r="AB31" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC31" s="48" t="s">
         <v>21</v>
@@ -6139,7 +6142,7 @@
       <c r="AJ31" s="48"/>
       <c r="AK31" s="48"/>
       <c r="AL31" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM31" s="48" t="s">
         <v>21</v>
@@ -6160,7 +6163,7 @@
     </row>
     <row r="32" spans="1:52" s="10" customFormat="1">
       <c r="A32" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B32" s="46">
         <v>31</v>
@@ -6176,13 +6179,13 @@
         <v>19</v>
       </c>
       <c r="G32" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H32" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I32" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J32" s="48" t="s">
         <v>18</v>
@@ -6205,13 +6208,13 @@
       <c r="Z32" s="48"/>
       <c r="AA32" s="48"/>
       <c r="AB32" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC32" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD32" s="48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AE32" s="48" t="s">
         <v>21</v>
@@ -6223,7 +6226,7 @@
       <c r="AJ32" s="48"/>
       <c r="AK32" s="48"/>
       <c r="AL32" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM32" s="48" t="s">
         <v>21</v>
@@ -6258,7 +6261,7 @@
         <v>19</v>
       </c>
       <c r="G33" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H33" s="52" t="s">
         <v>21</v>
@@ -6283,13 +6286,13 @@
       <c r="Z33" s="48"/>
       <c r="AA33" s="48"/>
       <c r="AB33" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC33" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD33" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE33" s="48" t="s">
         <v>21</v>
@@ -6332,7 +6335,7 @@
         <v>19</v>
       </c>
       <c r="G34" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H34" s="52" t="s">
         <v>18</v>
@@ -6367,7 +6370,7 @@
       <c r="AJ34" s="48"/>
       <c r="AK34" s="48"/>
       <c r="AL34" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM34" s="48" t="s">
         <v>21</v>
@@ -6402,13 +6405,13 @@
         <v>19</v>
       </c>
       <c r="G35" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H35" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I35" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J35" s="48" t="s">
         <v>18</v>
@@ -6417,7 +6420,7 @@
       <c r="L35" s="49"/>
       <c r="M35" s="48"/>
       <c r="N35" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O35" s="48" t="s">
         <v>18</v>
@@ -6476,7 +6479,7 @@
         <v>19</v>
       </c>
       <c r="G36" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H36" s="52" t="s">
         <v>18</v>
@@ -6487,7 +6490,7 @@
       <c r="L36" s="49"/>
       <c r="M36" s="48"/>
       <c r="N36" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O36" s="48" t="s">
         <v>21</v>
@@ -6515,7 +6518,7 @@
       <c r="AJ36" s="48"/>
       <c r="AK36" s="48"/>
       <c r="AL36" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM36" s="48" t="s">
         <v>21</v>
@@ -6550,7 +6553,7 @@
         <v>19</v>
       </c>
       <c r="G37" s="48" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H37" s="52" t="s">
         <v>18</v>
@@ -6616,7 +6619,7 @@
         <v>19</v>
       </c>
       <c r="G38" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H38" s="52" t="s">
         <v>18</v>
@@ -6651,7 +6654,7 @@
       <c r="AJ38" s="48"/>
       <c r="AK38" s="48"/>
       <c r="AL38" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM38" s="48" t="s">
         <v>21</v>
@@ -6686,7 +6689,7 @@
         <v>19</v>
       </c>
       <c r="G39" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H39" s="52" t="s">
         <v>18</v>
@@ -6711,13 +6714,13 @@
       <c r="Z39" s="48"/>
       <c r="AA39" s="48"/>
       <c r="AB39" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC39" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD39" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE39" s="48" t="s">
         <v>18</v>
@@ -6760,7 +6763,7 @@
         <v>19</v>
       </c>
       <c r="G40" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H40" s="52" t="s">
         <v>18</v>
@@ -6795,7 +6798,7 @@
       <c r="AJ40" s="48"/>
       <c r="AK40" s="48"/>
       <c r="AL40" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM40" s="48" t="s">
         <v>21</v>
@@ -6830,7 +6833,7 @@
         <v>19</v>
       </c>
       <c r="G41" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H41" s="52" t="s">
         <v>18</v>
@@ -6896,7 +6899,7 @@
         <v>19</v>
       </c>
       <c r="G42" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H42" s="52" t="s">
         <v>18</v>
@@ -6921,7 +6924,7 @@
       <c r="Z42" s="48"/>
       <c r="AA42" s="48"/>
       <c r="AB42" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC42" s="48" t="s">
         <v>18</v>
@@ -6956,7 +6959,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D43" s="47"/>
       <c r="E43" s="46" t="s">
@@ -6966,13 +6969,13 @@
         <v>19</v>
       </c>
       <c r="G43" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H43" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I43" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J43" s="48" t="s">
         <v>18</v>
@@ -6995,7 +6998,7 @@
       <c r="Z43" s="48"/>
       <c r="AA43" s="48"/>
       <c r="AB43" s="48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AC43" s="48" t="s">
         <v>21</v>
@@ -7009,7 +7012,7 @@
       <c r="AJ43" s="48"/>
       <c r="AK43" s="48"/>
       <c r="AL43" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM43" s="48" t="s">
         <v>21</v>
@@ -7034,7 +7037,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D44" s="47"/>
       <c r="E44" s="46" t="s">
@@ -7044,13 +7047,13 @@
         <v>19</v>
       </c>
       <c r="G44" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H44" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I44" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J44" s="48" t="s">
         <v>18</v>
@@ -7077,13 +7080,13 @@
       <c r="Z44" s="48"/>
       <c r="AA44" s="48"/>
       <c r="AB44" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC44" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD44" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE44" s="48" t="s">
         <v>18</v>
@@ -7116,7 +7119,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D45" s="47"/>
       <c r="E45" s="46" t="s">
@@ -7126,7 +7129,7 @@
         <v>19</v>
       </c>
       <c r="G45" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H45" s="52" t="s">
         <v>18</v>
@@ -7182,7 +7185,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D46" s="47"/>
       <c r="E46" s="46" t="s">
@@ -7192,7 +7195,7 @@
         <v>19</v>
       </c>
       <c r="G46" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H46" s="52" t="s">
         <v>18</v>
@@ -7248,7 +7251,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D47" s="47"/>
       <c r="E47" s="46" t="s">
@@ -7258,7 +7261,7 @@
         <v>19</v>
       </c>
       <c r="G47" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H47" s="52" t="s">
         <v>18</v>
@@ -7269,7 +7272,7 @@
       <c r="L47" s="49"/>
       <c r="M47" s="48"/>
       <c r="N47" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O47" s="48" t="s">
         <v>18</v>
@@ -7318,7 +7321,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D48" s="47"/>
       <c r="E48" s="46" t="s">
@@ -7328,7 +7331,7 @@
         <v>19</v>
       </c>
       <c r="G48" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H48" s="52" t="s">
         <v>18</v>
@@ -7384,7 +7387,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D49" s="47"/>
       <c r="E49" s="46" t="s">
@@ -7394,7 +7397,7 @@
         <v>19</v>
       </c>
       <c r="G49" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H49" s="52" t="s">
         <v>18</v>
@@ -7450,7 +7453,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D50" s="47"/>
       <c r="E50" s="46" t="s">
@@ -7460,13 +7463,13 @@
         <v>19</v>
       </c>
       <c r="G50" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H50" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I50" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J50" s="48" t="s">
         <v>18</v>
@@ -7493,13 +7496,13 @@
       <c r="Z50" s="48"/>
       <c r="AA50" s="48"/>
       <c r="AB50" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC50" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD50" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE50" s="48" t="s">
         <v>18</v>
@@ -7532,7 +7535,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D51" s="47"/>
       <c r="E51" s="46" t="s">
@@ -7542,7 +7545,7 @@
         <v>19</v>
       </c>
       <c r="G51" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H51" s="52" t="s">
         <v>18</v>
@@ -7598,7 +7601,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D52" s="47"/>
       <c r="E52" s="46" t="s">
@@ -7608,13 +7611,13 @@
         <v>19</v>
       </c>
       <c r="G52" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H52" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I52" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J52" s="48" t="s">
         <v>18</v>
@@ -7641,13 +7644,13 @@
       <c r="Z52" s="48"/>
       <c r="AA52" s="48"/>
       <c r="AB52" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC52" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD52" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AE52" s="48" t="s">
         <v>18</v>
@@ -7680,7 +7683,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D53" s="47"/>
       <c r="E53" s="46" t="s">
@@ -7690,7 +7693,7 @@
         <v>19</v>
       </c>
       <c r="G53" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H53" s="52" t="s">
         <v>18</v>
@@ -7701,7 +7704,7 @@
       <c r="L53" s="49"/>
       <c r="M53" s="48"/>
       <c r="N53" s="48" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O53" s="48" t="s">
         <v>18</v>
@@ -7750,7 +7753,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D54" s="47"/>
       <c r="E54" s="46" t="s">
@@ -7760,7 +7763,7 @@
         <v>19</v>
       </c>
       <c r="G54" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H54" s="52" t="s">
         <v>18</v>
@@ -7816,7 +7819,7 @@
         <v>54</v>
       </c>
       <c r="C55" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D55" s="47"/>
       <c r="E55" s="46" t="s">
@@ -7826,7 +7829,7 @@
         <v>19</v>
       </c>
       <c r="G55" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H55" s="52" t="s">
         <v>18</v>
@@ -7851,7 +7854,7 @@
       <c r="Z55" s="48"/>
       <c r="AA55" s="48"/>
       <c r="AB55" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC55" s="48" t="s">
         <v>18</v>
@@ -7886,7 +7889,7 @@
         <v>55</v>
       </c>
       <c r="C56" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D56" s="47"/>
       <c r="E56" s="46" t="s">
@@ -7896,7 +7899,7 @@
         <v>19</v>
       </c>
       <c r="G56" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H56" s="52" t="s">
         <v>18</v>
@@ -7952,7 +7955,7 @@
         <v>56</v>
       </c>
       <c r="C57" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D57" s="47"/>
       <c r="E57" s="46" t="s">
@@ -7962,7 +7965,7 @@
         <v>19</v>
       </c>
       <c r="G57" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H57" s="52" t="s">
         <v>18</v>
@@ -8028,7 +8031,7 @@
         <v>19</v>
       </c>
       <c r="G58" s="48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H58" s="52" t="s">
         <v>18</v>
@@ -8094,19 +8097,19 @@
         <v>19</v>
       </c>
       <c r="G59" s="48" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H59" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I59" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J59" s="48" t="s">
         <v>18</v>
       </c>
       <c r="K59" s="49" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L59" s="49"/>
       <c r="M59" s="48"/>
@@ -8129,19 +8132,19 @@
       <c r="Z59" s="48"/>
       <c r="AA59" s="48"/>
       <c r="AB59" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC59" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD59" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE59" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AF59" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AG59" s="48" t="s">
         <v>18</v>
@@ -8182,22 +8185,22 @@
         <v>19</v>
       </c>
       <c r="G60" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H60" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I60" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J60" s="48" t="s">
         <v>18</v>
       </c>
       <c r="K60" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L60" s="48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M60" s="48" t="s">
         <v>18</v>
@@ -8221,13 +8224,13 @@
       <c r="Z60" s="48"/>
       <c r="AA60" s="48"/>
       <c r="AB60" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC60" s="48" t="s">
         <v>18</v>
       </c>
       <c r="AD60" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE60" s="48" t="s">
         <v>18</v>
@@ -8260,7 +8263,7 @@
         <v>60</v>
       </c>
       <c r="C61" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D61" s="47"/>
       <c r="E61" s="46" t="s">
@@ -8270,13 +8273,13 @@
         <v>19</v>
       </c>
       <c r="G61" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H61" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I61" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J61" s="48" t="s">
         <v>18</v>
@@ -8285,7 +8288,7 @@
       <c r="L61" s="49"/>
       <c r="M61" s="48"/>
       <c r="N61" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O61" s="48" t="s">
         <v>18</v>
@@ -8313,7 +8316,7 @@
       <c r="AJ61" s="48"/>
       <c r="AK61" s="48"/>
       <c r="AL61" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM61" s="48" t="s">
         <v>18</v>
@@ -8338,7 +8341,7 @@
         <v>61</v>
       </c>
       <c r="C62" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D62" s="47"/>
       <c r="E62" s="46" t="s">
@@ -8348,7 +8351,7 @@
         <v>19</v>
       </c>
       <c r="G62" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H62" s="52" t="s">
         <v>18</v>
@@ -8414,13 +8417,13 @@
         <v>19</v>
       </c>
       <c r="G63" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H63" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I63" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J63" s="48" t="s">
         <v>18</v>
@@ -8429,7 +8432,7 @@
       <c r="L63" s="49"/>
       <c r="M63" s="48"/>
       <c r="N63" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O63" s="48" t="s">
         <v>18</v>
@@ -8478,7 +8481,7 @@
         <v>63</v>
       </c>
       <c r="C64" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D64" s="47"/>
       <c r="E64" s="46" t="s">
@@ -8488,7 +8491,7 @@
         <v>19</v>
       </c>
       <c r="G64" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H64" s="52" t="s">
         <v>18</v>
@@ -8499,7 +8502,7 @@
       <c r="L64" s="49"/>
       <c r="M64" s="48"/>
       <c r="N64" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O64" s="48" t="s">
         <v>18</v>
@@ -8548,7 +8551,7 @@
         <v>64</v>
       </c>
       <c r="C65" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D65" s="47"/>
       <c r="E65" s="46" t="s">
@@ -8558,7 +8561,7 @@
         <v>19</v>
       </c>
       <c r="G65" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H65" s="52" t="s">
         <v>18</v>
@@ -8614,7 +8617,7 @@
         <v>65</v>
       </c>
       <c r="C66" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D66" s="47"/>
       <c r="E66" s="46" t="s">
@@ -8624,7 +8627,7 @@
         <v>19</v>
       </c>
       <c r="G66" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H66" s="52" t="s">
         <v>18</v>
@@ -8680,7 +8683,7 @@
         <v>66</v>
       </c>
       <c r="C67" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D67" s="47"/>
       <c r="E67" s="46" t="s">
@@ -8690,7 +8693,7 @@
         <v>19</v>
       </c>
       <c r="G67" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H67" s="52" t="s">
         <v>18</v>
@@ -8746,7 +8749,7 @@
         <v>67</v>
       </c>
       <c r="C68" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D68" s="47"/>
       <c r="E68" s="46" t="s">
@@ -8756,7 +8759,7 @@
         <v>19</v>
       </c>
       <c r="G68" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H68" s="52" t="s">
         <v>18</v>
@@ -8822,7 +8825,7 @@
         <v>19</v>
       </c>
       <c r="G69" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H69" s="52" t="s">
         <v>18</v>
@@ -8878,7 +8881,7 @@
         <v>69</v>
       </c>
       <c r="C70" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D70" s="47"/>
       <c r="E70" s="46" t="s">
@@ -8888,7 +8891,7 @@
         <v>19</v>
       </c>
       <c r="G70" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H70" s="52" t="s">
         <v>18</v>
@@ -8944,7 +8947,7 @@
         <v>70</v>
       </c>
       <c r="C71" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D71" s="47"/>
       <c r="E71" s="46" t="s">
@@ -8954,7 +8957,7 @@
         <v>19</v>
       </c>
       <c r="G71" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H71" s="52" t="s">
         <v>18</v>
@@ -9010,7 +9013,7 @@
         <v>71</v>
       </c>
       <c r="C72" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D72" s="47"/>
       <c r="E72" s="46" t="s">
@@ -9020,7 +9023,7 @@
         <v>19</v>
       </c>
       <c r="G72" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H72" s="52" t="s">
         <v>18</v>
@@ -9076,7 +9079,7 @@
         <v>72</v>
       </c>
       <c r="C73" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D73" s="47"/>
       <c r="E73" s="46" t="s">
@@ -9086,7 +9089,7 @@
         <v>19</v>
       </c>
       <c r="G73" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H73" s="52" t="s">
         <v>18</v>
@@ -9152,7 +9155,7 @@
         <v>19</v>
       </c>
       <c r="G74" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H74" s="52" t="s">
         <v>18</v>
@@ -9208,7 +9211,7 @@
         <v>74</v>
       </c>
       <c r="C75" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D75" s="47"/>
       <c r="E75" s="46" t="s">
@@ -9218,7 +9221,7 @@
         <v>19</v>
       </c>
       <c r="G75" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H75" s="52" t="s">
         <v>18</v>
@@ -9274,7 +9277,7 @@
         <v>75</v>
       </c>
       <c r="C76" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D76" s="47"/>
       <c r="E76" s="46" t="s">
@@ -9284,7 +9287,7 @@
         <v>19</v>
       </c>
       <c r="G76" s="48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H76" s="52" t="s">
         <v>18</v>
@@ -9295,7 +9298,7 @@
       <c r="L76" s="49"/>
       <c r="M76" s="48"/>
       <c r="N76" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O76" s="48" t="s">
         <v>18</v>
@@ -9323,7 +9326,7 @@
       <c r="AJ76" s="48"/>
       <c r="AK76" s="48"/>
       <c r="AL76" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM76" s="48" t="s">
         <v>18</v>
@@ -9348,7 +9351,7 @@
         <v>76</v>
       </c>
       <c r="C77" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D77" s="47"/>
       <c r="E77" s="46" t="s">
@@ -9358,7 +9361,7 @@
         <v>19</v>
       </c>
       <c r="G77" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H77" s="52" t="s">
         <v>21</v>
@@ -9369,7 +9372,7 @@
       <c r="L77" s="49"/>
       <c r="M77" s="48"/>
       <c r="N77" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O77" s="48" t="s">
         <v>18</v>
@@ -9387,7 +9390,7 @@
       <c r="Z77" s="48"/>
       <c r="AA77" s="48"/>
       <c r="AB77" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC77" s="48" t="s">
         <v>21</v>
@@ -9432,7 +9435,7 @@
         <v>19</v>
       </c>
       <c r="G78" s="48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H78" s="52" t="s">
         <v>18</v>
@@ -9443,7 +9446,7 @@
       <c r="L78" s="49"/>
       <c r="M78" s="48"/>
       <c r="N78" s="52" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="O78" s="48" t="s">
         <v>18</v>
@@ -9502,7 +9505,7 @@
         <v>19</v>
       </c>
       <c r="G79" s="48" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H79" s="52" t="s">
         <v>18</v>
@@ -9568,13 +9571,13 @@
         <v>19</v>
       </c>
       <c r="G80" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H80" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I80" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J80" s="48" t="s">
         <v>18</v>
@@ -9638,7 +9641,7 @@
         <v>19</v>
       </c>
       <c r="G81" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H81" s="52" t="s">
         <v>18</v>
@@ -9704,7 +9707,7 @@
         <v>19</v>
       </c>
       <c r="G82" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H82" s="52" t="s">
         <v>21</v>
@@ -9715,7 +9718,7 @@
       <c r="L82" s="49"/>
       <c r="M82" s="48"/>
       <c r="N82" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O82" s="48" t="s">
         <v>18</v>
@@ -9733,7 +9736,7 @@
       <c r="Z82" s="48"/>
       <c r="AA82" s="48"/>
       <c r="AB82" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC82" s="48" t="s">
         <v>21</v>
@@ -9768,7 +9771,7 @@
         <v>87</v>
       </c>
       <c r="C83" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D83" s="47"/>
       <c r="E83" s="46" t="s">
@@ -9778,7 +9781,7 @@
         <v>19</v>
       </c>
       <c r="G83" s="48" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H83" s="52" t="s">
         <v>18</v>
@@ -9844,13 +9847,13 @@
         <v>19</v>
       </c>
       <c r="G84" s="48" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H84" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I84" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J84" s="48" t="s">
         <v>18</v>
@@ -9904,7 +9907,7 @@
         <v>89</v>
       </c>
       <c r="C85" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D85" s="47"/>
       <c r="E85" s="46" t="s">
@@ -9914,7 +9917,7 @@
         <v>19</v>
       </c>
       <c r="G85" s="48" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H85" s="52" t="s">
         <v>18</v>
@@ -9970,7 +9973,7 @@
         <v>102</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D86" s="47"/>
       <c r="E86" s="46" t="s">
@@ -9980,13 +9983,13 @@
         <v>19</v>
       </c>
       <c r="G86" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H86" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I86" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J86" s="48" t="s">
         <v>18</v>
@@ -9995,7 +9998,7 @@
       <c r="L86" s="49"/>
       <c r="M86" s="48"/>
       <c r="N86" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O86" s="48" t="s">
         <v>18</v>
@@ -10013,7 +10016,7 @@
       <c r="Z86" s="48"/>
       <c r="AA86" s="48"/>
       <c r="AB86" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC86" s="48" t="s">
         <v>21</v>
@@ -10027,7 +10030,7 @@
       <c r="AJ86" s="48"/>
       <c r="AK86" s="48"/>
       <c r="AL86" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM86" s="48" t="s">
         <v>18</v>
@@ -10052,7 +10055,7 @@
         <v>103</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D87" s="47"/>
       <c r="E87" s="46" t="s">
@@ -10062,13 +10065,13 @@
         <v>19</v>
       </c>
       <c r="G87" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H87" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I87" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J87" s="48" t="s">
         <v>18</v>
@@ -10077,7 +10080,7 @@
       <c r="L87" s="49"/>
       <c r="M87" s="48"/>
       <c r="N87" s="52" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="O87" s="48" t="s">
         <v>18</v>
@@ -10105,7 +10108,7 @@
       <c r="AJ87" s="48"/>
       <c r="AK87" s="48"/>
       <c r="AL87" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM87" s="48" t="s">
         <v>18</v>
@@ -10130,7 +10133,7 @@
         <v>104</v>
       </c>
       <c r="C88" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D88" s="47"/>
       <c r="E88" s="46" t="s">
@@ -10140,7 +10143,7 @@
         <v>19</v>
       </c>
       <c r="G88" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H88" s="52" t="s">
         <v>18</v>
@@ -10196,7 +10199,7 @@
         <v>105</v>
       </c>
       <c r="C89" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D89" s="47"/>
       <c r="E89" s="46" t="s">
@@ -10206,7 +10209,7 @@
         <v>19</v>
       </c>
       <c r="G89" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H89" s="52" t="s">
         <v>18</v>
@@ -10262,7 +10265,7 @@
         <v>106</v>
       </c>
       <c r="C90" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D90" s="47"/>
       <c r="E90" s="46" t="s">
@@ -10272,7 +10275,7 @@
         <v>19</v>
       </c>
       <c r="G90" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H90" s="52" t="s">
         <v>18</v>
@@ -10283,7 +10286,7 @@
       <c r="L90" s="49"/>
       <c r="M90" s="48"/>
       <c r="N90" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O90" s="48" t="s">
         <v>18</v>
@@ -10301,7 +10304,7 @@
       <c r="Z90" s="48"/>
       <c r="AA90" s="48"/>
       <c r="AB90" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC90" s="48" t="s">
         <v>21</v>
@@ -10336,7 +10339,7 @@
         <v>107</v>
       </c>
       <c r="C91" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D91" s="47"/>
       <c r="E91" s="46" t="s">
@@ -10346,7 +10349,7 @@
         <v>19</v>
       </c>
       <c r="G91" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H91" s="52" t="s">
         <v>18</v>
@@ -10402,7 +10405,7 @@
         <v>108</v>
       </c>
       <c r="C92" s="52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D92" s="47"/>
       <c r="E92" s="46" t="s">
@@ -10412,7 +10415,7 @@
         <v>19</v>
       </c>
       <c r="G92" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H92" s="52" t="s">
         <v>18</v>
@@ -10468,7 +10471,7 @@
         <v>111</v>
       </c>
       <c r="C93" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D93" s="47"/>
       <c r="E93" s="46" t="s">
@@ -10478,7 +10481,7 @@
         <v>19</v>
       </c>
       <c r="G93" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H93" s="52" t="s">
         <v>18</v>
@@ -10534,7 +10537,7 @@
         <v>116</v>
       </c>
       <c r="C94" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D94" s="47"/>
       <c r="E94" s="46" t="s">
@@ -10544,13 +10547,13 @@
         <v>19</v>
       </c>
       <c r="G94" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H94" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I94" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J94" s="48" t="s">
         <v>18</v>
@@ -10559,7 +10562,7 @@
       <c r="L94" s="49"/>
       <c r="M94" s="48"/>
       <c r="N94" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O94" s="48" t="s">
         <v>18</v>
@@ -10577,7 +10580,7 @@
       <c r="Z94" s="48"/>
       <c r="AA94" s="48"/>
       <c r="AB94" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC94" s="48" t="s">
         <v>21</v>
@@ -10612,7 +10615,7 @@
         <v>117</v>
       </c>
       <c r="C95" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D95" s="47"/>
       <c r="E95" s="46" t="s">
@@ -10622,13 +10625,13 @@
         <v>19</v>
       </c>
       <c r="G95" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H95" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I95" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J95" s="48" t="s">
         <v>18</v>
@@ -10637,7 +10640,7 @@
       <c r="L95" s="49"/>
       <c r="M95" s="48"/>
       <c r="N95" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O95" s="48" t="s">
         <v>21</v>
@@ -10665,7 +10668,7 @@
       <c r="AJ95" s="48"/>
       <c r="AK95" s="48"/>
       <c r="AL95" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM95" s="48" t="s">
         <v>21</v>
@@ -10700,7 +10703,7 @@
         <v>19</v>
       </c>
       <c r="G96" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H96" s="52" t="s">
         <v>18</v>
@@ -10766,13 +10769,13 @@
         <v>19</v>
       </c>
       <c r="G97" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H97" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I97" s="52" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J97" s="48" t="s">
         <v>18</v>
@@ -10781,7 +10784,7 @@
       <c r="L97" s="49"/>
       <c r="M97" s="48"/>
       <c r="N97" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O97" s="48" t="s">
         <v>18</v>
@@ -10789,13 +10792,13 @@
       <c r="P97" s="48"/>
       <c r="Q97" s="48"/>
       <c r="R97" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S97" s="48" t="s">
         <v>18</v>
       </c>
       <c r="T97" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="U97" s="48" t="s">
         <v>18</v>
@@ -10813,7 +10816,7 @@
       <c r="AF97" s="48"/>
       <c r="AG97" s="48"/>
       <c r="AH97" s="48" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AI97" s="48" t="s">
         <v>18</v>
@@ -10821,7 +10824,7 @@
       <c r="AJ97" s="48"/>
       <c r="AK97" s="48"/>
       <c r="AL97" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM97" s="48" t="s">
         <v>18</v>
@@ -10846,7 +10849,7 @@
         <v>120</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D98" s="47"/>
       <c r="E98" s="46" t="s">
@@ -10856,13 +10859,13 @@
         <v>19</v>
       </c>
       <c r="G98" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H98" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I98" s="48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J98" s="48" t="s">
         <v>18</v>
@@ -10889,7 +10892,7 @@
       <c r="Z98" s="48"/>
       <c r="AA98" s="48"/>
       <c r="AB98" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC98" s="48" t="s">
         <v>18</v>
@@ -10924,7 +10927,7 @@
         <v>121</v>
       </c>
       <c r="C99" s="52" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D99" s="47"/>
       <c r="E99" s="46" t="s">
@@ -10934,7 +10937,7 @@
         <v>19</v>
       </c>
       <c r="G99" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H99" s="52" t="s">
         <v>18</v>
@@ -11000,13 +11003,13 @@
         <v>19</v>
       </c>
       <c r="G100" s="48" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H100" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I100" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J100" s="48" t="s">
         <v>18</v>
@@ -11015,7 +11018,7 @@
       <c r="L100" s="49"/>
       <c r="M100" s="48"/>
       <c r="N100" s="52" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O100" s="48" t="s">
         <v>18</v>
@@ -11023,7 +11026,7 @@
       <c r="P100" s="48"/>
       <c r="Q100" s="48"/>
       <c r="R100" s="48" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="S100" s="48" t="s">
         <v>18</v>
@@ -11047,7 +11050,7 @@
       <c r="AJ100" s="48"/>
       <c r="AK100" s="48"/>
       <c r="AL100" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM100" s="48" t="s">
         <v>18</v>
@@ -11082,13 +11085,13 @@
         <v>19</v>
       </c>
       <c r="G101" s="48" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H101" s="52" t="s">
         <v>18</v>
       </c>
       <c r="I101" s="52" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J101" s="48" t="s">
         <v>18</v>
@@ -11097,7 +11100,7 @@
       <c r="L101" s="49"/>
       <c r="M101" s="48"/>
       <c r="N101" s="52" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O101" s="48" t="s">
         <v>18</v>
@@ -11125,7 +11128,7 @@
       <c r="AJ101" s="48"/>
       <c r="AK101" s="48"/>
       <c r="AL101" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM101" s="48" t="s">
         <v>18</v>
@@ -11160,7 +11163,7 @@
         <v>19</v>
       </c>
       <c r="G102" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H102" s="52" t="s">
         <v>21</v>
@@ -11171,7 +11174,7 @@
       <c r="L102" s="49"/>
       <c r="M102" s="48"/>
       <c r="N102" s="53" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O102" s="48" t="s">
         <v>18</v>
@@ -11189,7 +11192,7 @@
       <c r="Z102" s="48"/>
       <c r="AA102" s="48"/>
       <c r="AB102" s="48" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AC102" s="48" t="s">
         <v>18</v>
@@ -11203,7 +11206,7 @@
       <c r="AJ102" s="48"/>
       <c r="AK102" s="48"/>
       <c r="AL102" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM102" s="48" t="s">
         <v>21</v>
@@ -11238,7 +11241,7 @@
         <v>19</v>
       </c>
       <c r="G103" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H103" s="52" t="s">
         <v>21</v>
@@ -11263,7 +11266,7 @@
       <c r="Z103" s="48"/>
       <c r="AA103" s="48"/>
       <c r="AB103" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC103" s="48" t="s">
         <v>21</v>
@@ -11277,7 +11280,7 @@
       <c r="AJ103" s="48"/>
       <c r="AK103" s="48"/>
       <c r="AL103" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM103" s="48" t="s">
         <v>21</v>
@@ -11312,7 +11315,7 @@
         <v>19</v>
       </c>
       <c r="G104" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H104" s="52" t="s">
         <v>21</v>
@@ -11323,7 +11326,7 @@
       <c r="L104" s="49"/>
       <c r="M104" s="48"/>
       <c r="N104" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O104" s="48" t="s">
         <v>18</v>
@@ -11331,7 +11334,7 @@
       <c r="P104" s="48"/>
       <c r="Q104" s="48"/>
       <c r="R104" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S104" s="48" t="s">
         <v>21</v>
@@ -11355,7 +11358,7 @@
       <c r="AJ104" s="48"/>
       <c r="AK104" s="48"/>
       <c r="AL104" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM104" s="48" t="s">
         <v>21</v>
@@ -11365,7 +11368,7 @@
       <c r="AP104" s="48"/>
       <c r="AQ104" s="55"/>
       <c r="AR104" s="56" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AS104" s="13"/>
       <c r="AT104" s="13"/>
@@ -11392,13 +11395,13 @@
         <v>19</v>
       </c>
       <c r="G105" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H105" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I105" s="48" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J105" s="48" t="s">
         <v>21</v>
@@ -11407,7 +11410,7 @@
       <c r="L105" s="49"/>
       <c r="M105" s="48"/>
       <c r="N105" s="52" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O105" s="48" t="s">
         <v>21</v>
@@ -11415,7 +11418,7 @@
       <c r="P105" s="48"/>
       <c r="Q105" s="48"/>
       <c r="R105" s="48" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="S105" s="48" t="s">
         <v>21</v>
@@ -11439,7 +11442,7 @@
       <c r="AJ105" s="48"/>
       <c r="AK105" s="48"/>
       <c r="AL105" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM105" s="48" t="s">
         <v>21</v>
@@ -11474,7 +11477,7 @@
         <v>19</v>
       </c>
       <c r="G106" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H106" s="52" t="s">
         <v>21</v>
@@ -11509,7 +11512,7 @@
       <c r="AJ106" s="48"/>
       <c r="AK106" s="48"/>
       <c r="AL106" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM106" s="48" t="s">
         <v>21</v>
@@ -11544,7 +11547,7 @@
         <v>19</v>
       </c>
       <c r="G107" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H107" s="52" t="s">
         <v>21</v>
@@ -11569,19 +11572,19 @@
       <c r="Z107" s="48"/>
       <c r="AA107" s="48"/>
       <c r="AB107" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC107" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD107" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE107" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AF107" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AG107" s="48" t="s">
         <v>21</v>
@@ -11622,7 +11625,7 @@
         <v>19</v>
       </c>
       <c r="G108" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H108" s="52" t="s">
         <v>21</v>
@@ -11657,7 +11660,7 @@
       <c r="AJ108" s="48"/>
       <c r="AK108" s="48"/>
       <c r="AL108" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM108" s="48" t="s">
         <v>21</v>
@@ -11692,7 +11695,7 @@
         <v>19</v>
       </c>
       <c r="G109" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H109" s="52" t="s">
         <v>21</v>
@@ -11758,7 +11761,7 @@
         <v>19</v>
       </c>
       <c r="G110" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H110" s="52" t="s">
         <v>21</v>
@@ -11793,7 +11796,7 @@
       <c r="AJ110" s="48"/>
       <c r="AK110" s="48"/>
       <c r="AL110" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM110" s="48" t="s">
         <v>21</v>
@@ -11828,7 +11831,7 @@
         <v>19</v>
       </c>
       <c r="G111" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H111" s="52" t="s">
         <v>21</v>
@@ -11894,7 +11897,7 @@
         <v>19</v>
       </c>
       <c r="G112" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H112" s="52" t="s">
         <v>21</v>
@@ -11905,7 +11908,7 @@
       <c r="L112" s="49"/>
       <c r="M112" s="48"/>
       <c r="N112" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O112" s="48" t="s">
         <v>21</v>
@@ -11964,7 +11967,7 @@
         <v>19</v>
       </c>
       <c r="G113" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H113" s="52" t="s">
         <v>21</v>
@@ -11989,7 +11992,7 @@
       <c r="Z113" s="48"/>
       <c r="AA113" s="48"/>
       <c r="AB113" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC113" s="48" t="s">
         <v>21</v>
@@ -12034,7 +12037,7 @@
         <v>19</v>
       </c>
       <c r="G114" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H114" s="52" t="s">
         <v>21</v>
@@ -12059,7 +12062,7 @@
       <c r="Z114" s="48"/>
       <c r="AA114" s="48"/>
       <c r="AB114" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC114" s="48" t="s">
         <v>21</v>
@@ -12073,7 +12076,7 @@
       <c r="AJ114" s="48"/>
       <c r="AK114" s="48"/>
       <c r="AL114" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM114" s="48" t="s">
         <v>21</v>
@@ -12108,7 +12111,7 @@
         <v>19</v>
       </c>
       <c r="G115" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H115" s="52" t="s">
         <v>21</v>
@@ -12133,7 +12136,7 @@
       <c r="Z115" s="48"/>
       <c r="AA115" s="48"/>
       <c r="AB115" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC115" s="48" t="s">
         <v>21</v>
@@ -12178,7 +12181,7 @@
         <v>19</v>
       </c>
       <c r="G116" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H116" s="52" t="s">
         <v>21</v>
@@ -12203,7 +12206,7 @@
       <c r="Z116" s="48"/>
       <c r="AA116" s="48"/>
       <c r="AB116" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC116" s="48" t="s">
         <v>21</v>
@@ -12217,7 +12220,7 @@
       <c r="AJ116" s="48"/>
       <c r="AK116" s="48"/>
       <c r="AL116" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM116" s="48" t="s">
         <v>21</v>
@@ -12252,7 +12255,7 @@
         <v>19</v>
       </c>
       <c r="G117" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H117" s="52" t="s">
         <v>21</v>
@@ -12318,7 +12321,7 @@
         <v>19</v>
       </c>
       <c r="G118" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H118" s="52" t="s">
         <v>21</v>
@@ -12353,7 +12356,7 @@
       <c r="AJ118" s="48"/>
       <c r="AK118" s="48"/>
       <c r="AL118" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM118" s="48" t="s">
         <v>21</v>
@@ -12388,7 +12391,7 @@
         <v>19</v>
       </c>
       <c r="G119" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H119" s="52" t="s">
         <v>21</v>
@@ -12413,7 +12416,7 @@
       <c r="Z119" s="48"/>
       <c r="AA119" s="48"/>
       <c r="AB119" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC119" s="48" t="s">
         <v>21</v>
@@ -12458,7 +12461,7 @@
         <v>19</v>
       </c>
       <c r="G120" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H120" s="52" t="s">
         <v>21</v>
@@ -12493,7 +12496,7 @@
       <c r="AJ120" s="48"/>
       <c r="AK120" s="48"/>
       <c r="AL120" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM120" s="48" t="s">
         <v>21</v>
@@ -12528,7 +12531,7 @@
         <v>19</v>
       </c>
       <c r="G121" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H121" s="52" t="s">
         <v>21</v>
@@ -12594,7 +12597,7 @@
         <v>19</v>
       </c>
       <c r="G122" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H122" s="52" t="s">
         <v>21</v>
@@ -12605,7 +12608,7 @@
       <c r="L122" s="49"/>
       <c r="M122" s="48"/>
       <c r="N122" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O122" s="48" t="s">
         <v>21</v>
@@ -12623,13 +12626,13 @@
       <c r="Z122" s="48"/>
       <c r="AA122" s="48"/>
       <c r="AB122" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC122" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD122" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE122" s="48" t="s">
         <v>21</v>
@@ -12672,7 +12675,7 @@
         <v>19</v>
       </c>
       <c r="G123" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H123" s="52" t="s">
         <v>21</v>
@@ -12697,7 +12700,7 @@
       <c r="Z123" s="48"/>
       <c r="AA123" s="48"/>
       <c r="AB123" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC123" s="48" t="s">
         <v>21</v>
@@ -12742,7 +12745,7 @@
         <v>19</v>
       </c>
       <c r="G124" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H124" s="52" t="s">
         <v>21</v>
@@ -12767,7 +12770,7 @@
       <c r="Z124" s="48"/>
       <c r="AA124" s="48"/>
       <c r="AB124" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC124" s="48" t="s">
         <v>21</v>
@@ -12781,7 +12784,7 @@
       <c r="AJ124" s="48"/>
       <c r="AK124" s="48"/>
       <c r="AL124" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM124" s="48" t="s">
         <v>21</v>
@@ -12816,7 +12819,7 @@
         <v>19</v>
       </c>
       <c r="G125" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H125" s="52" t="s">
         <v>21</v>
@@ -12841,7 +12844,7 @@
       <c r="Z125" s="48"/>
       <c r="AA125" s="48"/>
       <c r="AB125" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC125" s="48" t="s">
         <v>21</v>
@@ -12886,7 +12889,7 @@
         <v>19</v>
       </c>
       <c r="G126" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H126" s="52" t="s">
         <v>21</v>
@@ -12911,13 +12914,13 @@
       <c r="Z126" s="48"/>
       <c r="AA126" s="48"/>
       <c r="AB126" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC126" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD126" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE126" s="48" t="s">
         <v>21</v>
@@ -12929,7 +12932,7 @@
       <c r="AJ126" s="48"/>
       <c r="AK126" s="48"/>
       <c r="AL126" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM126" s="48" t="s">
         <v>21</v>
@@ -12964,7 +12967,7 @@
         <v>19</v>
       </c>
       <c r="G127" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H127" s="52" t="s">
         <v>21</v>
@@ -13030,7 +13033,7 @@
         <v>19</v>
       </c>
       <c r="G128" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H128" s="52" t="s">
         <v>21</v>
@@ -13041,7 +13044,7 @@
       <c r="L128" s="49"/>
       <c r="M128" s="48"/>
       <c r="N128" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O128" s="48" t="s">
         <v>21</v>
@@ -13100,7 +13103,7 @@
         <v>19</v>
       </c>
       <c r="G129" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H129" s="52" t="s">
         <v>21</v>
@@ -13125,7 +13128,7 @@
       <c r="Z129" s="48"/>
       <c r="AA129" s="48"/>
       <c r="AB129" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC129" s="48" t="s">
         <v>21</v>
@@ -13170,7 +13173,7 @@
         <v>19</v>
       </c>
       <c r="G130" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H130" s="52" t="s">
         <v>21</v>
@@ -13195,7 +13198,7 @@
       <c r="Z130" s="48"/>
       <c r="AA130" s="48"/>
       <c r="AB130" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC130" s="48" t="s">
         <v>21</v>
@@ -13209,7 +13212,7 @@
       <c r="AJ130" s="48"/>
       <c r="AK130" s="48"/>
       <c r="AL130" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM130" s="48" t="s">
         <v>21</v>
@@ -13244,7 +13247,7 @@
         <v>19</v>
       </c>
       <c r="G131" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H131" s="52" t="s">
         <v>21</v>
@@ -13269,7 +13272,7 @@
       <c r="Z131" s="48"/>
       <c r="AA131" s="48"/>
       <c r="AB131" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC131" s="48" t="s">
         <v>21</v>
@@ -13314,7 +13317,7 @@
         <v>19</v>
       </c>
       <c r="G132" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H132" s="52" t="s">
         <v>21</v>
@@ -13339,7 +13342,7 @@
       <c r="Z132" s="48"/>
       <c r="AA132" s="48"/>
       <c r="AB132" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC132" s="48" t="s">
         <v>21</v>
@@ -13353,7 +13356,7 @@
       <c r="AJ132" s="48"/>
       <c r="AK132" s="48"/>
       <c r="AL132" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM132" s="48" t="s">
         <v>21</v>
@@ -13388,7 +13391,7 @@
         <v>19</v>
       </c>
       <c r="G133" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H133" s="52" t="s">
         <v>21</v>
@@ -13454,7 +13457,7 @@
         <v>19</v>
       </c>
       <c r="G134" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H134" s="52" t="s">
         <v>21</v>
@@ -13479,7 +13482,7 @@
       <c r="Z134" s="48"/>
       <c r="AA134" s="48"/>
       <c r="AB134" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC134" s="48" t="s">
         <v>21</v>
@@ -13524,7 +13527,7 @@
         <v>19</v>
       </c>
       <c r="G135" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H135" s="52" t="s">
         <v>21</v>
@@ -13549,7 +13552,7 @@
       <c r="Z135" s="48"/>
       <c r="AA135" s="48"/>
       <c r="AB135" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC135" s="48" t="s">
         <v>21</v>
@@ -13563,7 +13566,7 @@
       <c r="AJ135" s="48"/>
       <c r="AK135" s="48"/>
       <c r="AL135" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM135" s="48" t="s">
         <v>21</v>
@@ -13598,7 +13601,7 @@
         <v>19</v>
       </c>
       <c r="G136" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H136" s="52" t="s">
         <v>21</v>
@@ -13609,7 +13612,7 @@
       <c r="L136" s="49"/>
       <c r="M136" s="48"/>
       <c r="N136" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O136" s="48" t="s">
         <v>21</v>
@@ -13668,7 +13671,7 @@
         <v>19</v>
       </c>
       <c r="G137" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H137" s="52" t="s">
         <v>21</v>
@@ -13693,7 +13696,7 @@
       <c r="Z137" s="48"/>
       <c r="AA137" s="48"/>
       <c r="AB137" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC137" s="48" t="s">
         <v>21</v>
@@ -13707,7 +13710,7 @@
       <c r="AJ137" s="48"/>
       <c r="AK137" s="48"/>
       <c r="AL137" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM137" s="48" t="s">
         <v>21</v>
@@ -13742,7 +13745,7 @@
         <v>19</v>
       </c>
       <c r="G138" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H138" s="52" t="s">
         <v>21</v>
@@ -13767,7 +13770,7 @@
       <c r="Z138" s="48"/>
       <c r="AA138" s="48"/>
       <c r="AB138" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC138" s="48" t="s">
         <v>21</v>
@@ -13812,7 +13815,7 @@
         <v>19</v>
       </c>
       <c r="G139" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H139" s="52" t="s">
         <v>21</v>
@@ -13847,7 +13850,7 @@
       <c r="AJ139" s="48"/>
       <c r="AK139" s="48"/>
       <c r="AL139" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM139" s="48" t="s">
         <v>21</v>
@@ -13882,7 +13885,7 @@
         <v>19</v>
       </c>
       <c r="G140" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H140" s="52" t="s">
         <v>21</v>
@@ -13948,7 +13951,7 @@
         <v>19</v>
       </c>
       <c r="G141" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H141" s="52" t="s">
         <v>21</v>
@@ -13983,7 +13986,7 @@
       <c r="AJ141" s="48"/>
       <c r="AK141" s="48"/>
       <c r="AL141" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM141" s="48" t="s">
         <v>21</v>
@@ -14018,7 +14021,7 @@
         <v>19</v>
       </c>
       <c r="G142" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H142" s="52" t="s">
         <v>21</v>
@@ -14043,7 +14046,7 @@
       <c r="Z142" s="48"/>
       <c r="AA142" s="48"/>
       <c r="AB142" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC142" s="48" t="s">
         <v>21</v>
@@ -14088,7 +14091,7 @@
         <v>19</v>
       </c>
       <c r="G143" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H143" s="52" t="s">
         <v>21</v>
@@ -14123,7 +14126,7 @@
       <c r="AJ143" s="48"/>
       <c r="AK143" s="48"/>
       <c r="AL143" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM143" s="48" t="s">
         <v>21</v>
@@ -14158,7 +14161,7 @@
         <v>19</v>
       </c>
       <c r="G144" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H144" s="52" t="s">
         <v>21</v>
@@ -14183,7 +14186,7 @@
       <c r="Z144" s="48"/>
       <c r="AA144" s="48"/>
       <c r="AB144" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC144" s="48" t="s">
         <v>21</v>
@@ -14228,7 +14231,7 @@
         <v>19</v>
       </c>
       <c r="G145" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H145" s="52" t="s">
         <v>21</v>
@@ -14253,7 +14256,7 @@
       <c r="Z145" s="48"/>
       <c r="AA145" s="48"/>
       <c r="AB145" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC145" s="48" t="s">
         <v>21</v>
@@ -14267,7 +14270,7 @@
       <c r="AJ145" s="48"/>
       <c r="AK145" s="48"/>
       <c r="AL145" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM145" s="48" t="s">
         <v>21</v>
@@ -14302,7 +14305,7 @@
         <v>19</v>
       </c>
       <c r="G146" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H146" s="52" t="s">
         <v>21</v>
@@ -14327,7 +14330,7 @@
       <c r="Z146" s="48"/>
       <c r="AA146" s="48"/>
       <c r="AB146" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC146" s="48" t="s">
         <v>21</v>
@@ -14372,7 +14375,7 @@
         <v>19</v>
       </c>
       <c r="G147" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H147" s="52" t="s">
         <v>21</v>
@@ -14397,7 +14400,7 @@
       <c r="Z147" s="48"/>
       <c r="AA147" s="48"/>
       <c r="AB147" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC147" s="48" t="s">
         <v>21</v>
@@ -14411,7 +14414,7 @@
       <c r="AJ147" s="48"/>
       <c r="AK147" s="48"/>
       <c r="AL147" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM147" s="48" t="s">
         <v>21</v>
@@ -14446,7 +14449,7 @@
         <v>19</v>
       </c>
       <c r="G148" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H148" s="52" t="s">
         <v>21</v>
@@ -14471,7 +14474,7 @@
       <c r="Z148" s="48"/>
       <c r="AA148" s="48"/>
       <c r="AB148" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC148" s="48" t="s">
         <v>21</v>
@@ -14516,7 +14519,7 @@
         <v>19</v>
       </c>
       <c r="G149" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H149" s="52" t="s">
         <v>21</v>
@@ -14541,7 +14544,7 @@
       <c r="Z149" s="48"/>
       <c r="AA149" s="48"/>
       <c r="AB149" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC149" s="48" t="s">
         <v>21</v>
@@ -14555,7 +14558,7 @@
       <c r="AJ149" s="48"/>
       <c r="AK149" s="48"/>
       <c r="AL149" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM149" s="48" t="s">
         <v>21</v>
@@ -14590,7 +14593,7 @@
         <v>19</v>
       </c>
       <c r="G150" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H150" s="52" t="s">
         <v>21</v>
@@ -14615,7 +14618,7 @@
       <c r="Z150" s="48"/>
       <c r="AA150" s="48"/>
       <c r="AB150" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC150" s="48" t="s">
         <v>21</v>
@@ -14660,7 +14663,7 @@
         <v>19</v>
       </c>
       <c r="G151" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H151" s="52" t="s">
         <v>21</v>
@@ -14685,13 +14688,13 @@
       <c r="Z151" s="48"/>
       <c r="AA151" s="48"/>
       <c r="AB151" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC151" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD151" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE151" s="48" t="s">
         <v>21</v>
@@ -14703,7 +14706,7 @@
       <c r="AJ151" s="48"/>
       <c r="AK151" s="48"/>
       <c r="AL151" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM151" s="48" t="s">
         <v>21</v>
@@ -14738,7 +14741,7 @@
         <v>19</v>
       </c>
       <c r="G152" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H152" s="52" t="s">
         <v>21</v>
@@ -14804,7 +14807,7 @@
         <v>19</v>
       </c>
       <c r="G153" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H153" s="52" t="s">
         <v>21</v>
@@ -14815,7 +14818,7 @@
       <c r="L153" s="49"/>
       <c r="M153" s="48"/>
       <c r="N153" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O153" s="48" t="s">
         <v>21</v>
@@ -14874,7 +14877,7 @@
         <v>19</v>
       </c>
       <c r="G154" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H154" s="52" t="s">
         <v>21</v>
@@ -14940,7 +14943,7 @@
         <v>19</v>
       </c>
       <c r="G155" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H155" s="52" t="s">
         <v>21</v>
@@ -14975,7 +14978,7 @@
       <c r="AJ155" s="48"/>
       <c r="AK155" s="48"/>
       <c r="AL155" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM155" s="48" t="s">
         <v>21</v>
@@ -15010,7 +15013,7 @@
         <v>19</v>
       </c>
       <c r="G156" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H156" s="52" t="s">
         <v>21</v>
@@ -15035,7 +15038,7 @@
       <c r="Z156" s="48"/>
       <c r="AA156" s="48"/>
       <c r="AB156" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC156" s="48" t="s">
         <v>21</v>
@@ -15045,7 +15048,7 @@
       <c r="AF156" s="48"/>
       <c r="AG156" s="48"/>
       <c r="AH156" s="48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI156" s="48" t="s">
         <v>21</v>
@@ -15084,7 +15087,7 @@
         <v>19</v>
       </c>
       <c r="G157" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H157" s="52" t="s">
         <v>21</v>
@@ -15119,7 +15122,7 @@
       <c r="AJ157" s="48"/>
       <c r="AK157" s="48"/>
       <c r="AL157" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM157" s="48" t="s">
         <v>21</v>
@@ -15154,7 +15157,7 @@
         <v>19</v>
       </c>
       <c r="G158" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H158" s="52" t="s">
         <v>21</v>
@@ -15220,7 +15223,7 @@
         <v>19</v>
       </c>
       <c r="G159" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H159" s="52" t="s">
         <v>21</v>
@@ -15255,7 +15258,7 @@
       <c r="AJ159" s="48"/>
       <c r="AK159" s="48"/>
       <c r="AL159" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM159" s="48" t="s">
         <v>21</v>
@@ -15290,13 +15293,13 @@
         <v>19</v>
       </c>
       <c r="G160" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H160" s="52" t="s">
         <v>21</v>
       </c>
       <c r="I160" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J160" s="48" t="s">
         <v>21</v>
@@ -15360,7 +15363,7 @@
         <v>19</v>
       </c>
       <c r="G161" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H161" s="52" t="s">
         <v>21</v>
@@ -15385,7 +15388,7 @@
       <c r="Z161" s="48"/>
       <c r="AA161" s="48"/>
       <c r="AB161" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC161" s="48" t="s">
         <v>21</v>
@@ -15430,7 +15433,7 @@
         <v>19</v>
       </c>
       <c r="G162" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H162" s="52" t="s">
         <v>21</v>
@@ -15496,7 +15499,7 @@
         <v>19</v>
       </c>
       <c r="G163" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H163" s="52" t="s">
         <v>21</v>
@@ -15521,7 +15524,7 @@
       <c r="Z163" s="48"/>
       <c r="AA163" s="48"/>
       <c r="AB163" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC163" s="48" t="s">
         <v>21</v>
@@ -15535,7 +15538,7 @@
       <c r="AJ163" s="48"/>
       <c r="AK163" s="48"/>
       <c r="AL163" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM163" s="48" t="s">
         <v>21</v>
@@ -15570,7 +15573,7 @@
         <v>19</v>
       </c>
       <c r="G164" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H164" s="52" t="s">
         <v>21</v>
@@ -15636,7 +15639,7 @@
         <v>19</v>
       </c>
       <c r="G165" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H165" s="52" t="s">
         <v>21</v>
@@ -15661,7 +15664,7 @@
       <c r="Z165" s="48"/>
       <c r="AA165" s="48"/>
       <c r="AB165" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC165" s="48" t="s">
         <v>21</v>
@@ -15675,7 +15678,7 @@
       <c r="AJ165" s="48"/>
       <c r="AK165" s="48"/>
       <c r="AL165" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM165" s="48" t="s">
         <v>21</v>
@@ -15710,7 +15713,7 @@
         <v>19</v>
       </c>
       <c r="G166" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H166" s="52" t="s">
         <v>21</v>
@@ -15735,13 +15738,13 @@
       <c r="Z166" s="48"/>
       <c r="AA166" s="48"/>
       <c r="AB166" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC166" s="48" t="s">
         <v>21</v>
       </c>
       <c r="AD166" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AE166" s="48" t="s">
         <v>21</v>
@@ -15784,7 +15787,7 @@
         <v>19</v>
       </c>
       <c r="G167" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H167" s="52" t="s">
         <v>21</v>
@@ -15809,7 +15812,7 @@
       <c r="Z167" s="48"/>
       <c r="AA167" s="48"/>
       <c r="AB167" s="48" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AC167" s="48" t="s">
         <v>21</v>
@@ -15819,7 +15822,7 @@
       <c r="AF167" s="48"/>
       <c r="AG167" s="48"/>
       <c r="AH167" s="48" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AI167" s="48" t="s">
         <v>21</v>
@@ -15827,7 +15830,7 @@
       <c r="AJ167" s="48"/>
       <c r="AK167" s="48"/>
       <c r="AL167" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM167" s="48" t="s">
         <v>21</v>
@@ -15862,7 +15865,7 @@
         <v>19</v>
       </c>
       <c r="G168" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H168" s="52" t="s">
         <v>21</v>
@@ -15928,7 +15931,7 @@
         <v>19</v>
       </c>
       <c r="G169" s="48" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H169" s="52" t="s">
         <v>21</v>
@@ -15939,7 +15942,7 @@
       <c r="L169" s="49"/>
       <c r="M169" s="48"/>
       <c r="N169" s="48" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O169" s="48" t="s">
         <v>21</v>
@@ -15957,7 +15960,7 @@
       <c r="Z169" s="48"/>
       <c r="AA169" s="48"/>
       <c r="AB169" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC169" s="48" t="s">
         <v>21</v>
@@ -15971,7 +15974,7 @@
       <c r="AJ169" s="48"/>
       <c r="AK169" s="48"/>
       <c r="AL169" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM169" s="48" t="s">
         <v>21</v>
@@ -16006,7 +16009,7 @@
         <v>19</v>
       </c>
       <c r="G170" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H170" s="52" t="s">
         <v>21</v>
@@ -16031,7 +16034,7 @@
       <c r="Z170" s="48"/>
       <c r="AA170" s="48"/>
       <c r="AB170" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC170" s="48" t="s">
         <v>21</v>
@@ -16076,7 +16079,7 @@
         <v>19</v>
       </c>
       <c r="G171" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H171" s="52" t="s">
         <v>21</v>
@@ -16101,7 +16104,7 @@
       <c r="Z171" s="48"/>
       <c r="AA171" s="48"/>
       <c r="AB171" s="48" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AC171" s="48" t="s">
         <v>21</v>
@@ -16115,7 +16118,7 @@
       <c r="AJ171" s="48"/>
       <c r="AK171" s="48"/>
       <c r="AL171" s="48" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AM171" s="48" t="s">
         <v>21</v>
@@ -16150,7 +16153,7 @@
         <v>19</v>
       </c>
       <c r="G172" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H172" s="52" t="s">
         <v>21</v>
@@ -16175,7 +16178,7 @@
       <c r="Z172" s="48"/>
       <c r="AA172" s="48"/>
       <c r="AB172" s="48" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AC172" s="48" t="s">
         <v>21</v>
@@ -16220,7 +16223,7 @@
         <v>19</v>
       </c>
       <c r="G173" s="48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H173" s="52" t="s">
         <v>21</v>
@@ -16231,7 +16234,7 @@
       <c r="L173" s="49"/>
       <c r="M173" s="48"/>
       <c r="N173" s="48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O173" s="48" t="s">
         <v>21</v>
@@ -16259,7 +16262,7 @@
       <c r="AJ173" s="48"/>
       <c r="AK173" s="48"/>
       <c r="AL173" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AM173" s="48" t="s">
         <v>21</v>
@@ -16294,7 +16297,7 @@
         <v>19</v>
       </c>
       <c r="G174" s="48" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H174" s="52" t="s">
         <v>21</v>

</xml_diff>